<commit_message>
small change on importing the libraries and modules
</commit_message>
<xml_diff>
--- a/CVX_Kenya/New Code/sens_Productivity increase due to 100% new machines (not spoiling the cerry)/case_0.005.xlsx
+++ b/CVX_Kenya/New Code/sens_Productivity increase due to 100% new machines (not spoiling the cerry)/case_0.005.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payam\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\New Code\sens_Productivity increase due to 100% new machines (not spoiling the cerry)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE277DE-164E-461B-82E0-0FC59F609FA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC9DA02-02F7-47A2-A300-7B855B95CFA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="1" r:id="rId1"/>

</xml_diff>